<commit_message>
customer account updated with common error resolution
</commit_message>
<xml_diff>
--- a/Reconciliation_Report/Kohala_Zipline/Invoice.xlsx
+++ b/Reconciliation_Report/Kohala_Zipline/Invoice.xlsx
@@ -1,25 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://isscindia-my.sharepoint.com/personal/dixitp_issc_co_in/Documents/Dixit_Work/Hawaii_Forest_Trail/Reconciliation_Report/Kohala_Zipline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_F25DC773A252ABDACC10482769D87F385BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEFE9FE3-9F8D-4E86-8DA0-A8ECFEC3ABF1}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_F25DC773A252ABDACC10482769D87F385BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1162C1A7-FFAF-464F-B2BC-D7B29D13DC69}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="1" r:id="rId1"/>
     <sheet name="Invoice_Line" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -905,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BL19"/>
+  <dimension ref="A1:BM19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S19" sqref="S2:S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -930,55 +941,56 @@
     <col min="15" max="15" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="39" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="37.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="63.77734375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="28" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="50.6640625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="45.109375" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="52.44140625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="39" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="63.77734375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="28" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1033,146 +1045,146 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>0</v>
       </c>
@@ -1227,33 +1239,34 @@
       <c r="R2">
         <v>749504</v>
       </c>
-      <c r="S2" s="1">
+      <c r="S2" t="str">
+        <f>_xlfn.CONCAT("'",R2,"'",",")</f>
+        <v>'749504',</v>
+      </c>
+      <c r="T2" s="1">
         <v>45658</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>69</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>70</v>
       </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
       <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
         <v>74</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>71</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>6075</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>72</v>
       </c>
-      <c r="AA2" t="s">
-        <v>73</v>
-      </c>
       <c r="AB2" t="s">
         <v>73</v>
       </c>
@@ -1272,38 +1285,38 @@
       <c r="AG2" t="s">
         <v>73</v>
       </c>
-      <c r="AH2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>73</v>
+      <c r="AH2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI2" t="b">
+        <v>0</v>
       </c>
       <c r="AJ2" t="s">
         <v>73</v>
       </c>
-      <c r="AK2" s="1">
+      <c r="AK2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL2" s="1">
         <v>45658</v>
       </c>
-      <c r="AL2">
+      <c r="AM2">
         <v>2000</v>
       </c>
-      <c r="AM2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>74</v>
+      <c r="AN2" t="b">
+        <v>0</v>
       </c>
       <c r="AO2" t="s">
         <v>74</v>
       </c>
       <c r="AP2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ2">
-        <v>0</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
       </c>
       <c r="AS2" t="s">
         <v>73</v>
@@ -1365,8 +1378,11 @@
       <c r="BL2" t="s">
         <v>73</v>
       </c>
+      <c r="BM2" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -1421,99 +1437,100 @@
       <c r="R3">
         <v>770126</v>
       </c>
-      <c r="S3" s="1">
+      <c r="S3" t="str">
+        <f t="shared" ref="S3:S19" si="0">_xlfn.CONCAT("'",R3,"'",",")</f>
+        <v>'770126',</v>
+      </c>
+      <c r="T3" s="1">
         <v>45672</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>69</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>70</v>
       </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
       <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
         <v>293</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>76</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>6120</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>76</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>77</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>78</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <v>222</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>77</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>79</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>80</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>96740</v>
       </c>
-      <c r="AH3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI3">
+      <c r="AI3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
         <v>8</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>81</v>
       </c>
-      <c r="AK3" s="1">
+      <c r="AL3" s="1">
         <v>45702</v>
       </c>
-      <c r="AL3">
+      <c r="AM3">
         <v>4828.6499999999996</v>
       </c>
-      <c r="AM3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>74</v>
+      <c r="AN3" t="b">
+        <v>0</v>
       </c>
       <c r="AO3" t="s">
         <v>74</v>
       </c>
       <c r="AP3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ3" t="s">
         <v>82</v>
       </c>
-      <c r="AQ3">
+      <c r="AR3">
         <v>4828.6499999999996</v>
       </c>
-      <c r="AR3">
+      <c r="AS3">
         <v>99</v>
       </c>
-      <c r="AS3" t="s">
-        <v>73</v>
-      </c>
       <c r="AT3" t="s">
         <v>73</v>
       </c>
       <c r="AU3" t="s">
         <v>73</v>
       </c>
-      <c r="AV3">
+      <c r="AV3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AW3">
         <v>678289949</v>
       </c>
-      <c r="AW3" t="s">
-        <v>73</v>
-      </c>
       <c r="AX3" t="s">
         <v>73</v>
       </c>
@@ -1559,8 +1576,11 @@
       <c r="BL3" t="s">
         <v>73</v>
       </c>
+      <c r="BM3" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -1615,87 +1635,88 @@
       <c r="R4">
         <v>770125</v>
       </c>
-      <c r="S4" s="1">
+      <c r="S4" t="str">
+        <f t="shared" si="0"/>
+        <v>'770125',</v>
+      </c>
+      <c r="T4" s="1">
         <v>45672</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>69</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>70</v>
       </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
       <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
         <v>257</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>83</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>6119</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>84</v>
       </c>
-      <c r="AA4" t="s">
-        <v>73</v>
-      </c>
       <c r="AB4" t="s">
         <v>73</v>
       </c>
-      <c r="AC4">
+      <c r="AC4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD4">
         <v>210</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>84</v>
       </c>
-      <c r="AE4" t="s">
-        <v>73</v>
-      </c>
       <c r="AF4" t="s">
         <v>73</v>
       </c>
       <c r="AG4" t="s">
         <v>73</v>
       </c>
-      <c r="AH4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI4">
+      <c r="AH4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ4">
         <v>8</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>81</v>
       </c>
-      <c r="AK4" s="1">
+      <c r="AL4" s="1">
         <v>45702</v>
       </c>
-      <c r="AL4">
+      <c r="AM4">
         <v>3553.03</v>
       </c>
-      <c r="AM4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>74</v>
+      <c r="AN4" t="b">
+        <v>0</v>
       </c>
       <c r="AO4" t="s">
         <v>74</v>
       </c>
       <c r="AP4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ4" t="s">
         <v>85</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>3553.03</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>99</v>
       </c>
-      <c r="AS4" t="s">
-        <v>73</v>
-      </c>
       <c r="AT4" t="s">
         <v>73</v>
       </c>
@@ -1753,8 +1774,11 @@
       <c r="BL4" t="s">
         <v>73</v>
       </c>
+      <c r="BM4" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A5" t="b">
         <v>0</v>
       </c>
@@ -1809,87 +1833,88 @@
       <c r="R5">
         <v>770124</v>
       </c>
-      <c r="S5" s="1">
+      <c r="S5" t="str">
+        <f t="shared" si="0"/>
+        <v>'770124',</v>
+      </c>
+      <c r="T5" s="1">
         <v>45672</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>69</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>70</v>
       </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
       <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
         <v>49</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>86</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>6118</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>87</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>88</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>89</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>105</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>88</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>90</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>91</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>94105</v>
       </c>
-      <c r="AH5" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI5">
+      <c r="AI5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ5">
         <v>8</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>81</v>
       </c>
-      <c r="AK5" s="1">
+      <c r="AL5" s="1">
         <v>45702</v>
       </c>
-      <c r="AL5">
+      <c r="AM5">
         <v>6946.17</v>
       </c>
-      <c r="AM5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>74</v>
+      <c r="AN5" t="b">
+        <v>0</v>
       </c>
       <c r="AO5" t="s">
         <v>74</v>
       </c>
       <c r="AP5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ5" t="s">
         <v>92</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>6946.17</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>99</v>
       </c>
-      <c r="AS5" t="s">
-        <v>73</v>
-      </c>
       <c r="AT5" t="s">
         <v>73</v>
       </c>
@@ -1947,8 +1972,11 @@
       <c r="BL5" t="s">
         <v>73</v>
       </c>
+      <c r="BM5" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
         <v>0</v>
       </c>
@@ -2003,87 +2031,88 @@
       <c r="R6">
         <v>770123</v>
       </c>
-      <c r="S6" s="1">
+      <c r="S6" t="str">
+        <f t="shared" si="0"/>
+        <v>'770123',</v>
+      </c>
+      <c r="T6" s="1">
         <v>45672</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>69</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>70</v>
       </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
       <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
         <v>237</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>93</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>6117</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>94</v>
       </c>
-      <c r="AA6" t="s">
-        <v>73</v>
-      </c>
       <c r="AB6" t="s">
         <v>73</v>
       </c>
-      <c r="AC6">
+      <c r="AC6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD6">
         <v>204</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>94</v>
       </c>
-      <c r="AE6" t="s">
-        <v>73</v>
-      </c>
       <c r="AF6" t="s">
         <v>73</v>
       </c>
       <c r="AG6" t="s">
         <v>73</v>
       </c>
-      <c r="AH6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>73</v>
+      <c r="AH6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI6" t="b">
+        <v>1</v>
       </c>
       <c r="AJ6" t="s">
         <v>73</v>
       </c>
-      <c r="AK6" s="1">
+      <c r="AK6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL6" s="1">
         <v>45672</v>
       </c>
-      <c r="AL6">
+      <c r="AM6">
         <v>393.72</v>
       </c>
-      <c r="AM6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>74</v>
+      <c r="AN6" t="b">
+        <v>0</v>
       </c>
       <c r="AO6" t="s">
         <v>74</v>
       </c>
       <c r="AP6" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ6" t="s">
         <v>95</v>
       </c>
-      <c r="AQ6">
-        <v>0</v>
-      </c>
       <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
         <v>99</v>
       </c>
-      <c r="AS6" t="s">
-        <v>73</v>
-      </c>
       <c r="AT6" t="s">
         <v>73</v>
       </c>
@@ -2141,8 +2170,11 @@
       <c r="BL6" t="s">
         <v>73</v>
       </c>
+      <c r="BM6" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -2197,87 +2229,88 @@
       <c r="R7">
         <v>770122</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S7" t="str">
+        <f t="shared" si="0"/>
+        <v>'770122',</v>
+      </c>
+      <c r="T7" s="1">
         <v>45672</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>69</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>70</v>
       </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
       <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
         <v>213</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>96</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>6116</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>97</v>
       </c>
-      <c r="AA7" t="s">
-        <v>73</v>
-      </c>
       <c r="AB7" t="s">
         <v>73</v>
       </c>
-      <c r="AC7">
+      <c r="AC7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD7">
         <v>198</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>97</v>
       </c>
-      <c r="AE7" t="s">
-        <v>73</v>
-      </c>
       <c r="AF7" t="s">
         <v>73</v>
       </c>
       <c r="AG7" t="s">
         <v>73</v>
       </c>
-      <c r="AH7" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI7">
+      <c r="AH7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ7">
         <v>8</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AK7" t="s">
         <v>81</v>
       </c>
-      <c r="AK7" s="1">
+      <c r="AL7" s="1">
         <v>45702</v>
       </c>
-      <c r="AL7">
+      <c r="AM7">
         <v>2490.98</v>
       </c>
-      <c r="AM7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>74</v>
+      <c r="AN7" t="b">
+        <v>0</v>
       </c>
       <c r="AO7" t="s">
         <v>74</v>
       </c>
       <c r="AP7" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ7">
-        <v>0</v>
+        <v>74</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>73</v>
       </c>
       <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
         <v>99</v>
       </c>
-      <c r="AS7" t="s">
-        <v>73</v>
-      </c>
       <c r="AT7" t="s">
         <v>73</v>
       </c>
@@ -2335,8 +2368,11 @@
       <c r="BL7" t="s">
         <v>73</v>
       </c>
+      <c r="BM7" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A8" t="b">
         <v>0</v>
       </c>
@@ -2391,93 +2427,94 @@
       <c r="R8">
         <v>770121</v>
       </c>
-      <c r="S8" s="1">
+      <c r="S8" t="str">
+        <f t="shared" si="0"/>
+        <v>'770121',</v>
+      </c>
+      <c r="T8" s="1">
         <v>45672</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>69</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>70</v>
       </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
       <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
         <v>68</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>98</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>6115</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>99</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>100</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>101</v>
       </c>
-      <c r="AC8">
+      <c r="AD8">
         <v>125</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
         <v>99</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AF8" t="s">
         <v>102</v>
       </c>
-      <c r="AF8" t="s">
+      <c r="AG8" t="s">
         <v>80</v>
       </c>
-      <c r="AG8">
+      <c r="AH8">
         <v>96814</v>
       </c>
-      <c r="AH8" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>73</v>
+      <c r="AI8" t="b">
+        <v>1</v>
       </c>
       <c r="AJ8" t="s">
         <v>73</v>
       </c>
-      <c r="AK8" s="1">
+      <c r="AK8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL8" s="1">
         <v>45672</v>
       </c>
-      <c r="AL8">
+      <c r="AM8">
         <v>1513.6</v>
       </c>
-      <c r="AM8" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN8" t="s">
-        <v>74</v>
+      <c r="AN8" t="b">
+        <v>0</v>
       </c>
       <c r="AO8" t="s">
         <v>74</v>
       </c>
       <c r="AP8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ8" t="s">
         <v>103</v>
       </c>
-      <c r="AQ8">
+      <c r="AR8">
         <v>1513.6</v>
       </c>
-      <c r="AR8">
+      <c r="AS8">
         <v>99</v>
       </c>
-      <c r="AS8" t="s">
-        <v>73</v>
-      </c>
       <c r="AT8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU8" t="s">
         <v>100</v>
       </c>
-      <c r="AU8" t="s">
-        <v>73</v>
-      </c>
       <c r="AV8" t="s">
         <v>73</v>
       </c>
@@ -2529,8 +2566,11 @@
       <c r="BL8" t="s">
         <v>73</v>
       </c>
+      <c r="BM8" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A9" t="b">
         <v>0</v>
       </c>
@@ -2585,27 +2625,28 @@
       <c r="R9">
         <v>770120</v>
       </c>
-      <c r="S9" s="1">
+      <c r="S9" t="str">
+        <f t="shared" si="0"/>
+        <v>'770120',</v>
+      </c>
+      <c r="T9" s="1">
         <v>45672</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>69</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>70</v>
       </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
       <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
         <v>244</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>104</v>
       </c>
-      <c r="Y9" t="s">
-        <v>73</v>
-      </c>
       <c r="Z9" t="s">
         <v>73</v>
       </c>
@@ -2630,42 +2671,42 @@
       <c r="AG9" t="s">
         <v>73</v>
       </c>
-      <c r="AH9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI9">
+      <c r="AH9" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
         <v>8</v>
       </c>
-      <c r="AJ9" t="s">
+      <c r="AK9" t="s">
         <v>81</v>
       </c>
-      <c r="AK9" s="1">
+      <c r="AL9" s="1">
         <v>45702</v>
       </c>
-      <c r="AL9">
+      <c r="AM9">
         <v>390.03</v>
       </c>
-      <c r="AM9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN9" t="s">
-        <v>74</v>
+      <c r="AN9" t="b">
+        <v>0</v>
       </c>
       <c r="AO9" t="s">
         <v>74</v>
       </c>
       <c r="AP9" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ9">
+        <v>74</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR9">
         <v>390.03</v>
       </c>
-      <c r="AR9">
+      <c r="AS9">
         <v>99</v>
       </c>
-      <c r="AS9" t="s">
-        <v>73</v>
-      </c>
       <c r="AT9" t="s">
         <v>73</v>
       </c>
@@ -2723,8 +2764,11 @@
       <c r="BL9" t="s">
         <v>73</v>
       </c>
+      <c r="BM9" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -2779,93 +2823,94 @@
       <c r="R10">
         <v>770119</v>
       </c>
-      <c r="S10" s="1">
+      <c r="S10" t="str">
+        <f t="shared" si="0"/>
+        <v>'770119',</v>
+      </c>
+      <c r="T10" s="1">
         <v>45672</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>69</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>70</v>
       </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
       <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
         <v>148</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>105</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>6114</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AA10" t="s">
         <v>106</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AB10" t="s">
         <v>107</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
         <v>108</v>
       </c>
-      <c r="AC10">
+      <c r="AD10">
         <v>169</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AE10" t="s">
         <v>106</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AF10" t="s">
         <v>109</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AG10" t="s">
         <v>80</v>
       </c>
-      <c r="AG10">
+      <c r="AH10">
         <v>96761</v>
       </c>
-      <c r="AH10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI10">
+      <c r="AI10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ10">
         <v>8</v>
       </c>
-      <c r="AJ10" t="s">
+      <c r="AK10" t="s">
         <v>81</v>
       </c>
-      <c r="AK10" s="1">
+      <c r="AL10" s="1">
         <v>45702</v>
       </c>
-      <c r="AL10">
+      <c r="AM10">
         <v>548.70000000000005</v>
       </c>
-      <c r="AM10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN10" t="s">
-        <v>74</v>
+      <c r="AN10" t="b">
+        <v>0</v>
       </c>
       <c r="AO10" t="s">
         <v>74</v>
       </c>
       <c r="AP10" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ10" t="s">
         <v>110</v>
       </c>
-      <c r="AQ10">
+      <c r="AR10">
         <v>548.70000000000005</v>
       </c>
-      <c r="AR10">
+      <c r="AS10">
         <v>99</v>
       </c>
-      <c r="AS10" t="s">
-        <v>73</v>
-      </c>
       <c r="AT10" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU10" t="s">
         <v>107</v>
       </c>
-      <c r="AU10" t="s">
-        <v>73</v>
-      </c>
       <c r="AV10" t="s">
         <v>73</v>
       </c>
@@ -2917,8 +2962,11 @@
       <c r="BL10" t="s">
         <v>73</v>
       </c>
+      <c r="BM10" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A11" t="b">
         <v>0</v>
       </c>
@@ -2973,102 +3021,103 @@
       <c r="R11">
         <v>770118</v>
       </c>
-      <c r="S11" s="1">
+      <c r="S11" t="str">
+        <f t="shared" si="0"/>
+        <v>'770118',</v>
+      </c>
+      <c r="T11" s="1">
         <v>45672</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>69</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>70</v>
       </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
       <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
         <v>6</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>111</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>6113</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AA11" t="s">
         <v>112</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AB11" t="s">
         <v>113</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>114</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <v>62</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>112</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AF11" t="s">
         <v>115</v>
       </c>
-      <c r="AF11" t="s">
+      <c r="AG11" t="s">
         <v>80</v>
       </c>
-      <c r="AG11">
+      <c r="AH11">
         <v>96738</v>
       </c>
-      <c r="AH11" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI11">
+      <c r="AI11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ11">
         <v>19</v>
       </c>
-      <c r="AJ11" t="s">
+      <c r="AK11" t="s">
         <v>116</v>
       </c>
-      <c r="AK11" s="1">
+      <c r="AL11" s="1">
         <v>45717</v>
       </c>
-      <c r="AL11">
+      <c r="AM11">
         <v>1821.95</v>
       </c>
-      <c r="AM11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>74</v>
+      <c r="AN11" t="b">
+        <v>0</v>
       </c>
       <c r="AO11" t="s">
         <v>74</v>
       </c>
       <c r="AP11" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ11" t="s">
         <v>117</v>
       </c>
-      <c r="AQ11">
+      <c r="AR11">
         <v>1821.95</v>
       </c>
-      <c r="AR11">
+      <c r="AS11">
         <v>99</v>
       </c>
-      <c r="AS11" t="s">
-        <v>73</v>
-      </c>
       <c r="AT11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU11" t="s">
         <v>118</v>
       </c>
-      <c r="AU11" t="s">
-        <v>73</v>
-      </c>
       <c r="AV11" t="s">
         <v>73</v>
       </c>
       <c r="AW11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX11" t="s">
         <v>119</v>
       </c>
-      <c r="AX11" t="s">
-        <v>73</v>
-      </c>
       <c r="AY11" t="s">
         <v>73</v>
       </c>
@@ -3111,8 +3160,11 @@
       <c r="BL11" t="s">
         <v>73</v>
       </c>
+      <c r="BM11" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A12" t="b">
         <v>0</v>
       </c>
@@ -3167,87 +3219,88 @@
       <c r="R12">
         <v>770116</v>
       </c>
-      <c r="S12" s="1">
+      <c r="S12" t="str">
+        <f t="shared" si="0"/>
+        <v>'770116',</v>
+      </c>
+      <c r="T12" s="1">
         <v>45672</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>69</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>70</v>
       </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
       <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
         <v>28</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>120</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <v>6112</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AA12" t="s">
         <v>121</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AB12" t="s">
         <v>122</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AC12" t="s">
         <v>123</v>
       </c>
-      <c r="AC12">
+      <c r="AD12">
         <v>84</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>122</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AF12" t="s">
         <v>124</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AG12" t="s">
         <v>125</v>
       </c>
-      <c r="AG12">
+      <c r="AH12">
         <v>29485</v>
       </c>
-      <c r="AH12" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI12">
+      <c r="AI12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ12">
         <v>8</v>
       </c>
-      <c r="AJ12" t="s">
+      <c r="AK12" t="s">
         <v>81</v>
       </c>
-      <c r="AK12" s="1">
+      <c r="AL12" s="1">
         <v>45702</v>
       </c>
-      <c r="AL12">
+      <c r="AM12">
         <v>820.94</v>
       </c>
-      <c r="AM12" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN12" t="s">
-        <v>74</v>
+      <c r="AN12" t="b">
+        <v>0</v>
       </c>
       <c r="AO12" t="s">
         <v>74</v>
       </c>
       <c r="AP12" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ12" t="s">
         <v>126</v>
       </c>
-      <c r="AQ12">
+      <c r="AR12">
         <v>820.94</v>
       </c>
-      <c r="AR12">
+      <c r="AS12">
         <v>99</v>
       </c>
-      <c r="AS12" t="s">
-        <v>73</v>
-      </c>
       <c r="AT12" t="s">
         <v>73</v>
       </c>
@@ -3305,8 +3358,11 @@
       <c r="BL12" t="s">
         <v>73</v>
       </c>
+      <c r="BM12" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A13" t="b">
         <v>0</v>
       </c>
@@ -3361,87 +3417,88 @@
       <c r="R13">
         <v>770114</v>
       </c>
-      <c r="S13" s="1">
+      <c r="S13" t="str">
+        <f t="shared" si="0"/>
+        <v>'770114',</v>
+      </c>
+      <c r="T13" s="1">
         <v>45672</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>69</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
         <v>70</v>
       </c>
-      <c r="V13">
-        <v>0</v>
-      </c>
       <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
         <v>199</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Y13" t="s">
         <v>127</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <v>6111</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="AA13" t="s">
         <v>128</v>
       </c>
-      <c r="AA13" t="s">
-        <v>73</v>
-      </c>
       <c r="AB13" t="s">
         <v>73</v>
       </c>
-      <c r="AC13">
+      <c r="AC13" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD13">
         <v>189</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AE13" t="s">
         <v>128</v>
       </c>
-      <c r="AE13" t="s">
-        <v>73</v>
-      </c>
       <c r="AF13" t="s">
         <v>73</v>
       </c>
       <c r="AG13" t="s">
         <v>73</v>
       </c>
-      <c r="AH13" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI13">
+      <c r="AH13" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ13">
         <v>8</v>
       </c>
-      <c r="AJ13" t="s">
+      <c r="AK13" t="s">
         <v>81</v>
       </c>
-      <c r="AK13" s="1">
+      <c r="AL13" s="1">
         <v>45702</v>
       </c>
-      <c r="AL13">
+      <c r="AM13">
         <v>2115.17</v>
       </c>
-      <c r="AM13" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN13" t="s">
-        <v>74</v>
+      <c r="AN13" t="b">
+        <v>0</v>
       </c>
       <c r="AO13" t="s">
         <v>74</v>
       </c>
       <c r="AP13" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ13" t="s">
         <v>129</v>
       </c>
-      <c r="AQ13">
+      <c r="AR13">
         <v>2115.17</v>
       </c>
-      <c r="AR13">
+      <c r="AS13">
         <v>99</v>
       </c>
-      <c r="AS13" t="s">
-        <v>73</v>
-      </c>
       <c r="AT13" t="s">
         <v>73</v>
       </c>
@@ -3499,8 +3556,11 @@
       <c r="BL13" t="s">
         <v>73</v>
       </c>
+      <c r="BM13" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A14" t="b">
         <v>0</v>
       </c>
@@ -3555,93 +3615,94 @@
       <c r="R14">
         <v>770113</v>
       </c>
-      <c r="S14" s="1">
+      <c r="S14" t="str">
+        <f t="shared" si="0"/>
+        <v>'770113',</v>
+      </c>
+      <c r="T14" s="1">
         <v>45672</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>69</v>
       </c>
-      <c r="U14" t="s">
+      <c r="V14" t="s">
         <v>70</v>
       </c>
-      <c r="V14">
-        <v>0</v>
-      </c>
       <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
         <v>165</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Y14" t="s">
         <v>130</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
         <v>6110</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AA14" t="s">
         <v>131</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AB14" t="s">
         <v>132</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AC14" t="s">
         <v>133</v>
       </c>
-      <c r="AC14">
+      <c r="AD14">
         <v>173</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AE14" t="s">
         <v>131</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AF14" t="s">
         <v>134</v>
       </c>
-      <c r="AF14" t="s">
+      <c r="AG14" t="s">
         <v>135</v>
       </c>
-      <c r="AG14">
+      <c r="AH14">
         <v>65803</v>
       </c>
-      <c r="AH14" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI14">
+      <c r="AI14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ14">
         <v>8</v>
       </c>
-      <c r="AJ14" t="s">
+      <c r="AK14" t="s">
         <v>81</v>
       </c>
-      <c r="AK14" s="1">
+      <c r="AL14" s="1">
         <v>45702</v>
       </c>
-      <c r="AL14">
+      <c r="AM14">
         <v>255.23</v>
       </c>
-      <c r="AM14" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN14" t="s">
-        <v>74</v>
+      <c r="AN14" t="b">
+        <v>0</v>
       </c>
       <c r="AO14" t="s">
         <v>74</v>
       </c>
       <c r="AP14" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ14" t="s">
         <v>136</v>
       </c>
-      <c r="AQ14">
+      <c r="AR14">
         <v>255.23</v>
       </c>
-      <c r="AR14">
+      <c r="AS14">
         <v>99</v>
       </c>
-      <c r="AS14" t="s">
-        <v>73</v>
-      </c>
       <c r="AT14" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU14" t="s">
         <v>132</v>
       </c>
-      <c r="AU14" t="s">
-        <v>73</v>
-      </c>
       <c r="AV14" t="s">
         <v>73</v>
       </c>
@@ -3693,8 +3754,11 @@
       <c r="BL14" t="s">
         <v>73</v>
       </c>
+      <c r="BM14" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -3749,27 +3813,28 @@
       <c r="R15">
         <v>770111</v>
       </c>
-      <c r="S15" s="1">
+      <c r="S15" t="str">
+        <f t="shared" si="0"/>
+        <v>'770111',</v>
+      </c>
+      <c r="T15" s="1">
         <v>45672</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>69</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>70</v>
       </c>
-      <c r="V15">
-        <v>0</v>
-      </c>
       <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
         <v>239</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Y15" t="s">
         <v>137</v>
       </c>
-      <c r="Y15" t="s">
-        <v>73</v>
-      </c>
       <c r="Z15" t="s">
         <v>73</v>
       </c>
@@ -3794,42 +3859,42 @@
       <c r="AG15" t="s">
         <v>73</v>
       </c>
-      <c r="AH15" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI15">
+      <c r="AH15" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ15">
         <v>8</v>
       </c>
-      <c r="AJ15" t="s">
+      <c r="AK15" t="s">
         <v>81</v>
       </c>
-      <c r="AK15" s="1">
+      <c r="AL15" s="1">
         <v>45702</v>
       </c>
-      <c r="AL15">
+      <c r="AM15">
         <v>369.1</v>
       </c>
-      <c r="AM15" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN15" t="s">
-        <v>74</v>
+      <c r="AN15" t="b">
+        <v>0</v>
       </c>
       <c r="AO15" t="s">
         <v>74</v>
       </c>
       <c r="AP15" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ15" t="s">
         <v>138</v>
       </c>
-      <c r="AQ15">
+      <c r="AR15">
         <v>369.1</v>
       </c>
-      <c r="AR15">
+      <c r="AS15">
         <v>99</v>
       </c>
-      <c r="AS15" t="s">
-        <v>73</v>
-      </c>
       <c r="AT15" t="s">
         <v>73</v>
       </c>
@@ -3887,8 +3952,11 @@
       <c r="BL15" t="s">
         <v>73</v>
       </c>
+      <c r="BM15" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -3943,84 +4011,85 @@
       <c r="R16">
         <v>770127</v>
       </c>
-      <c r="S16" s="1">
+      <c r="S16" t="str">
+        <f t="shared" si="0"/>
+        <v>'770127',</v>
+      </c>
+      <c r="T16" s="1">
         <v>45678</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>69</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>70</v>
       </c>
-      <c r="V16">
-        <v>0</v>
-      </c>
       <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
         <v>3</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Y16" t="s">
         <v>140</v>
       </c>
-      <c r="Y16">
+      <c r="Z16">
         <v>6121</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="AA16" t="s">
         <v>141</v>
       </c>
-      <c r="AA16" t="s">
-        <v>73</v>
-      </c>
       <c r="AB16" t="s">
         <v>73</v>
       </c>
-      <c r="AC16">
+      <c r="AC16" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD16">
         <v>59</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AE16" t="s">
         <v>141</v>
       </c>
-      <c r="AE16" t="s">
-        <v>73</v>
-      </c>
       <c r="AF16" t="s">
         <v>73</v>
       </c>
       <c r="AG16" t="s">
         <v>73</v>
       </c>
-      <c r="AH16" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI16">
+      <c r="AH16" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ16">
         <v>8</v>
       </c>
-      <c r="AJ16" t="s">
+      <c r="AK16" t="s">
         <v>81</v>
       </c>
-      <c r="AK16" s="1">
+      <c r="AL16" s="1">
         <v>45708</v>
       </c>
-      <c r="AL16">
+      <c r="AM16">
         <v>942.99</v>
       </c>
-      <c r="AM16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN16" t="s">
-        <v>74</v>
+      <c r="AN16" t="b">
+        <v>0</v>
       </c>
       <c r="AO16" t="s">
         <v>74</v>
       </c>
       <c r="AP16" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ16" t="s">
         <v>142</v>
       </c>
-      <c r="AQ16">
+      <c r="AR16">
         <v>942.99</v>
       </c>
-      <c r="AR16" t="s">
-        <v>73</v>
-      </c>
       <c r="AS16" t="s">
         <v>73</v>
       </c>
@@ -4081,8 +4150,11 @@
       <c r="BL16" t="s">
         <v>73</v>
       </c>
+      <c r="BM16" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A17" t="b">
         <v>0</v>
       </c>
@@ -4137,33 +4209,34 @@
       <c r="R17">
         <v>756248</v>
       </c>
-      <c r="S17" s="1">
+      <c r="S17" t="str">
+        <f t="shared" si="0"/>
+        <v>'756248',</v>
+      </c>
+      <c r="T17" s="1">
         <v>45686</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>69</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>70</v>
       </c>
-      <c r="V17">
-        <v>0</v>
-      </c>
       <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
         <v>267</v>
       </c>
-      <c r="X17" t="s">
+      <c r="Y17" t="s">
         <v>144</v>
       </c>
-      <c r="Y17">
+      <c r="Z17">
         <v>6094</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AA17" t="s">
         <v>144</v>
       </c>
-      <c r="AA17" t="s">
-        <v>73</v>
-      </c>
       <c r="AB17" t="s">
         <v>73</v>
       </c>
@@ -4182,42 +4255,42 @@
       <c r="AG17" t="s">
         <v>73</v>
       </c>
-      <c r="AH17" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>73</v>
+      <c r="AH17" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI17" t="b">
+        <v>0</v>
       </c>
       <c r="AJ17" t="s">
         <v>73</v>
       </c>
-      <c r="AK17" s="1">
+      <c r="AK17" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL17" s="1">
         <v>45686</v>
       </c>
-      <c r="AL17">
+      <c r="AM17">
         <v>1885.99</v>
       </c>
-      <c r="AM17" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN17" t="s">
-        <v>74</v>
+      <c r="AN17" t="b">
+        <v>0</v>
       </c>
       <c r="AO17" t="s">
         <v>74</v>
       </c>
       <c r="AP17" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ17">
-        <v>0</v>
+        <v>74</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>73</v>
       </c>
       <c r="AR17">
+        <v>0</v>
+      </c>
+      <c r="AS17">
         <v>99</v>
       </c>
-      <c r="AS17" t="s">
-        <v>73</v>
-      </c>
       <c r="AT17" t="s">
         <v>73</v>
       </c>
@@ -4261,11 +4334,11 @@
         <v>73</v>
       </c>
       <c r="BH17" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI17" t="s">
         <v>145</v>
       </c>
-      <c r="BI17" t="s">
-        <v>73</v>
-      </c>
       <c r="BJ17" t="s">
         <v>73</v>
       </c>
@@ -4275,8 +4348,11 @@
       <c r="BL17" t="s">
         <v>73</v>
       </c>
+      <c r="BM17" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -4331,33 +4407,34 @@
       <c r="R18" t="s">
         <v>147</v>
       </c>
-      <c r="S18" s="1">
+      <c r="S18" t="str">
+        <f t="shared" si="0"/>
+        <v>'770128-C',</v>
+      </c>
+      <c r="T18" s="1">
         <v>45689</v>
       </c>
-      <c r="T18" t="s">
+      <c r="U18" t="s">
         <v>69</v>
       </c>
-      <c r="U18" t="s">
+      <c r="V18" t="s">
         <v>70</v>
       </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
       <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
         <v>74</v>
       </c>
-      <c r="X18" t="s">
+      <c r="Y18" t="s">
         <v>71</v>
       </c>
-      <c r="Y18">
+      <c r="Z18">
         <v>6122</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="AA18" t="s">
         <v>72</v>
       </c>
-      <c r="AA18" t="s">
-        <v>73</v>
-      </c>
       <c r="AB18" t="s">
         <v>73</v>
       </c>
@@ -4376,39 +4453,39 @@
       <c r="AG18" t="s">
         <v>73</v>
       </c>
-      <c r="AH18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI18" t="s">
-        <v>73</v>
+      <c r="AH18" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI18" t="b">
+        <v>0</v>
       </c>
       <c r="AJ18" t="s">
         <v>73</v>
       </c>
-      <c r="AK18" s="1">
+      <c r="AK18" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL18" s="1">
         <v>45689</v>
       </c>
-      <c r="AL18">
+      <c r="AM18">
         <v>2000</v>
       </c>
-      <c r="AM18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN18" t="s">
-        <v>74</v>
+      <c r="AN18" t="b">
+        <v>0</v>
       </c>
       <c r="AO18" t="s">
         <v>74</v>
       </c>
       <c r="AP18" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ18">
+        <v>74</v>
+      </c>
+      <c r="AQ18" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR18">
         <v>2000</v>
       </c>
-      <c r="AR18" t="s">
-        <v>73</v>
-      </c>
       <c r="AS18" t="s">
         <v>73</v>
       </c>
@@ -4469,8 +4546,11 @@
       <c r="BL18" t="s">
         <v>73</v>
       </c>
+      <c r="BM18" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -4525,33 +4605,34 @@
       <c r="R19" t="s">
         <v>149</v>
       </c>
-      <c r="S19" s="1">
+      <c r="S19" t="str">
+        <f t="shared" si="0"/>
+        <v>'770129-C',</v>
+      </c>
+      <c r="T19" s="1">
         <v>45717</v>
       </c>
-      <c r="T19" t="s">
+      <c r="U19" t="s">
         <v>69</v>
       </c>
-      <c r="U19" t="s">
+      <c r="V19" t="s">
         <v>70</v>
       </c>
-      <c r="V19">
-        <v>0</v>
-      </c>
       <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
         <v>74</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Y19" t="s">
         <v>71</v>
       </c>
-      <c r="Y19">
+      <c r="Z19">
         <v>6123</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="AA19" t="s">
         <v>72</v>
       </c>
-      <c r="AA19" t="s">
-        <v>73</v>
-      </c>
       <c r="AB19" t="s">
         <v>73</v>
       </c>
@@ -4570,39 +4651,39 @@
       <c r="AG19" t="s">
         <v>73</v>
       </c>
-      <c r="AH19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI19" t="s">
-        <v>73</v>
+      <c r="AH19" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI19" t="b">
+        <v>0</v>
       </c>
       <c r="AJ19" t="s">
         <v>73</v>
       </c>
-      <c r="AK19" s="1">
+      <c r="AK19" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL19" s="1">
         <v>45717</v>
       </c>
-      <c r="AL19">
+      <c r="AM19">
         <v>2000</v>
       </c>
-      <c r="AM19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN19" t="s">
-        <v>74</v>
+      <c r="AN19" t="b">
+        <v>0</v>
       </c>
       <c r="AO19" t="s">
         <v>74</v>
       </c>
       <c r="AP19" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ19">
+        <v>74</v>
+      </c>
+      <c r="AQ19" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR19">
         <v>2000</v>
       </c>
-      <c r="AR19" t="s">
-        <v>73</v>
-      </c>
       <c r="AS19" t="s">
         <v>73</v>
       </c>
@@ -4661,6 +4742,9 @@
         <v>73</v>
       </c>
       <c r="BL19" t="s">
+        <v>73</v>
+      </c>
+      <c r="BM19" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4673,8 +4757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5550D246-081D-4C43-9689-77EA56C361CC}">
   <dimension ref="A1:X40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:X40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>